<commit_message>
Clean up python script; output in kbps instead of raw bytes; other changes
</commit_message>
<xml_diff>
--- a/python/syntax_elements.xlsx
+++ b/python/syntax_elements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="241">
   <si>
     <t>NAL_UNIT_TOTAL_BODY</t>
   </si>
@@ -738,6 +738,15 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Prediction</t>
   </si>
 </sst>
 </file>
@@ -781,22 +790,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -812,12 +838,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C193" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C193" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:C193"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Syntax Element" dataDxfId="0"/>
+    <tableColumn id="1" name="Syntax Element" dataDxfId="1"/>
     <tableColumn id="2" name="Purpose Within Stream"/>
-    <tableColumn id="3" name="Category"/>
+    <tableColumn id="3" name="Category" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1091,1175 +1117,1431 @@
   </sheetPr>
   <dimension ref="A1:C465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="2" max="2" width="77.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>196</v>
       </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="C16" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C17" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="C18" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="C19" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C20" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="C21" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="C22" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="C23" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="C24" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="C25" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="C26" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="C27" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="C28" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="C29" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="C30" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="C31" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="C32" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="C33" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="C41" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="C42" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="C43" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="C44" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="C82" s="3"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="C90" s="3"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="C94" s="3"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="C96" s="3"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="C97" s="3"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="C98" s="3"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="C100" s="3"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="C101" s="3"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="C104" s="3"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="C105" s="3"/>
+    </row>
+    <row r="106" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="C110" s="3"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="C112" s="3"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="C113" s="3"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="C114" s="3"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="C115" s="3"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="C116" s="3"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="C117" s="3"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="C120" s="3"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="C121" s="3"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="C125" s="3"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="C126" s="3"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="C127" s="3"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="C128" s="3"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="C129" s="3"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="C131" s="3"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="C132" s="3"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+      <c r="C133" s="3"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="C134" s="3"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="C135" s="3"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="C136" s="3"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="C137" s="3"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+      <c r="C139" s="3"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+      <c r="C140" s="3"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+      <c r="C141" s="3"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
+      <c r="C142" s="3"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+      <c r="C143" s="3"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+      <c r="C144" s="3"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+      <c r="C145" s="3"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+      <c r="C146" s="3"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="6" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="6" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="6" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="6" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
+      <c r="C158" s="3"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="6" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
+      <c r="C159" s="3"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="6" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
+      <c r="C160" s="3"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="6" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
+      <c r="C161" s="3"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
+      <c r="C162" s="3"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="6" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
+      <c r="C163" s="3"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
+      <c r="C164" s="3"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
+      <c r="C165" s="3"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
+      <c r="C166" s="3"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="6" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
+      <c r="C167" s="3"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
+      <c r="C168" s="3"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
+      <c r="C169" s="3"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
+      <c r="C170" s="3"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
+      <c r="C171" s="3"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
+      <c r="C172" s="3"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
+      <c r="C173" s="3"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
+      <c r="C174" s="3"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
+      <c r="C175" s="3"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="6" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
+      <c r="C176" s="3"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="6" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
+      <c r="C177" s="3"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
+      <c r="C178" s="3"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
+      <c r="C179" s="3"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="6" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
+      <c r="C180" s="3"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="6" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="1" t="s">
+      <c r="C181" s="3"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
+      <c r="C182" s="3"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="1" t="s">
+      <c r="C183" s="3"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="6" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="1" t="s">
+      <c r="C184" s="3"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="6" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="1" t="s">
+      <c r="C185" s="3"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="6" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
+      <c r="C186" s="3"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
+      <c r="C187" s="3"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="6" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
+      <c r="C188" s="3"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
+      <c r="C189" s="3"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
+      <c r="C190" s="3"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="6" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
+      <c r="C191" s="3"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
+      <c r="C192" s="3"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C193" s="3"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>